<commit_message>
04: Delete unnecessary file
</commit_message>
<xml_diff>
--- a/04_XPS/xps.xlsx
+++ b/04_XPS/xps.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Desktop\XPS\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75203518-F1C9-4894-9E03-5C77FE4CC1E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-12015" yWindow="3165" windowWidth="21600" windowHeight="11385" xr2:uid="{3B4D2CC4-5008-41D5-BD68-513CF8DC95F6}"/>
+    <workbookView xWindow="-12015" yWindow="3165" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,14 +29,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -57,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>C1s</t>
   </si>
@@ -108,12 +102,30 @@
   </si>
   <si>
     <t>vazba</t>
+  </si>
+  <si>
+    <t>c-c nebo c-h</t>
+  </si>
+  <si>
+    <t>C-O</t>
+  </si>
+  <si>
+    <t>C=O</t>
+  </si>
+  <si>
+    <t>Al</t>
+  </si>
+  <si>
+    <t>Al2O3</t>
+  </si>
+  <si>
+    <t>Al(OH)3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -162,7 +174,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -220,7 +232,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -272,7 +284,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -466,18 +478,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A21BF53C-4AB8-41FE-97E8-134C23AD68CE}">
-  <dimension ref="A1:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,7 +497,7 @@
     <col min="4" max="4" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>12</v>
       </c>
@@ -502,7 +514,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -520,7 +532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -538,7 +550,7 @@
         <v>2.93</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -556,7 +568,7 @@
         <v>0.53700000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -574,7 +586,7 @@
         <v>5.07</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -592,7 +604,7 @@
         <v>0.81699999999999995</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -606,8 +618,11 @@
         <f>C7/SUM($C$7:$C$10)*100</f>
         <v>89.075038930721291</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -621,8 +636,11 @@
         <f t="shared" ref="D8:D10" si="0">C8/SUM($C$7:$C$10)*100</f>
         <v>5.3066035779207397</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -637,7 +655,7 @@
         <v>2.6124925798744463</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -651,8 +669,11 @@
         <f t="shared" si="0"/>
         <v>3.0058649114835219</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -666,8 +687,17 @@
         <f>C11/SUM($C$11:$C$13)*100</f>
         <v>12.791565046576014</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>72.8</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11">
+        <v>72.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -681,8 +711,15 @@
         <f t="shared" ref="D12:D13" si="1">C12/SUM($C$11:$C$13)*100</f>
         <v>7.0192758148540593</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12">
+        <f>B12-(B$11-G$11)</f>
+        <v>73.209999999999994</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -695,6 +732,16 @@
       <c r="D13" s="2">
         <f t="shared" si="1"/>
         <v>80.189159138569934</v>
+      </c>
+      <c r="E13">
+        <v>74.5</v>
+      </c>
+      <c r="F13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13">
+        <f>B13-(B$11-G$11)</f>
+        <v>74.77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>